<commit_message>
Adding help file for Deidentifier.
</commit_message>
<xml_diff>
--- a/DECS Excel Add-Ins/test files/dummy_data_extracted.xlsx
+++ b/DECS Excel Add-Ins/test files/dummy_data_extracted.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DECS-Office-AddIns\DECS Excel Add-Ins\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBF405CB-85C5-4813-977D-9A2A4626CD7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC3808F-4A2D-4610-A9BC-539409D82141}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21465" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21465" windowHeight="8790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
-    <sheet name="Labs" sheetId="2" r:id="rId2"/>
+    <sheet name="MRNs only" sheetId="3" r:id="rId2"/>
+    <sheet name="Labs" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>MRN</t>
   </si>
@@ -72,7 +73,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0#######"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +91,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -111,10 +122,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -122,11 +136,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="CenteredHeadings" xfId="1" xr:uid="{4FF51D72-895A-4B21-A520-186996EE926D}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FFD3D3D3"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFD3D3D3"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -426,140 +470,211 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="120.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="57.5703125" style="4" customWidth="1"/>
+    <col min="6" max="7" width="6.7109375" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1234</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="6">
         <v>36519</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="7">
         <v>81</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="7">
         <v>1013.2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>2354</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="6">
         <v>45414</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="7">
         <v>1234.5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>3456</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>34700</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>4567</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="7">
         <v>99.9</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="7">
         <v>1234.5999999999999</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>2354</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>45017</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="7">
         <v>1234.5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"NULL"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A3B116-6F3F-4435-82E8-FEAAE0132414}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1234</v>
+      </c>
+      <c r="B2" s="8"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2354</v>
+      </c>
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3456</v>
+      </c>
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4567</v>
+      </c>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>2354</v>
+      </c>
+      <c r="B6" s="8"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:B1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"NULL"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA3A826-9B8D-4E37-8CFF-3AC9A5AFB1E7}">
   <dimension ref="A1:C4"/>
   <sheetViews>

</xml_diff>